<commit_message>
Adding new featre, deleteing the student row for the given roll no
</commit_message>
<xml_diff>
--- a/data/leave_records.xlsx
+++ b/data/leave_records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -512,13 +512,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -535,17 +535,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>rahul111@gmail.com</t>
+          <t>nikhilside72@gmail.com</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -553,20 +553,20 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Anikit</t>
+          <t>Nikhil Maddheshiya</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ankit@gmail.com</t>
+          <t>nikhilmaddheshiya7275@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -580,20 +580,20 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nikhil Maddheshiya</t>
+          <t>demoname</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>nikhilmaddheshiya7275@gmail.com</t>
+          <t>demoname123@gmail.com</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -607,20 +607,20 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>demoname</t>
+          <t>Aashish</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>demoname123@gmail.com</t>
+          <t>ashimrt50@gmail.com</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -629,87 +629,6 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>112</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Prakrity Maddheshiya</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>prakrityiitjee2025@gmail.com</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>120</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>shub</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>subh123@gmail.com</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>123</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Aashish</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>ashimrt50@gmail.com</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>